<commit_message>
Update BOM and firmware
Comment out DEBUG define in FW
Update costing in BOM
Correct quantities, etc in BOM
</commit_message>
<xml_diff>
--- a/RGB-IR Backlight 7x7/Electrical/7inLED-cntr-J010130C.xlsx
+++ b/RGB-IR Backlight 7x7/Electrical/7inLED-cntr-J010130C.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawtelles\Documents\GitHub\RGB-IR LED Boards\RGB-IR Backlight 7x7\Electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2552043-8D4A-489A-A1B8-A2F5BAF09C21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF0DE76-560C-47A0-ACC2-BEA305DF5392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1035" yWindow="1440" windowWidth="25005" windowHeight="14250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="1755" windowWidth="32385" windowHeight="14445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="7inLED-cntr-J010130A" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="123">
   <si>
     <t>Qty</t>
   </si>
@@ -402,6 +402,9 @@
   </si>
   <si>
     <t>Plug in after board is complete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTAL </t>
   </si>
 </sst>
 </file>
@@ -954,9 +957,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -994,7 +997,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1100,7 +1103,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1242,7 +1245,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1253,10 +1256,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1920,6 +1923,15 @@
         <v>121</v>
       </c>
     </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>122</v>
+      </c>
+      <c r="I32" s="3">
+        <f>SUM(I4:I29)</f>
+        <v>90.11</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>